<commit_message>
Added testcase for different signings for experiment.
</commit_message>
<xml_diff>
--- a/src/test/java/config/testdata.xlsx
+++ b/src/test/java/config/testdata.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="14355" windowHeight="4695"/>
+    <workbookView xWindow="360" yWindow="105" windowWidth="14355" windowHeight="4695" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="users" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="SigningExperiment" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>George.PJacob@Perkinelmer.com</t>
   </si>
@@ -28,6 +28,30 @@
   </si>
   <si>
     <t>Password</t>
+  </si>
+  <si>
+    <t>Signing types</t>
+  </si>
+  <si>
+    <t>Experiment Sign</t>
+  </si>
+  <si>
+    <t>Sign and close</t>
+  </si>
+  <si>
+    <t>Type 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type 2 </t>
+  </si>
+  <si>
+    <t>Sign and add reviewers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type 3 </t>
+  </si>
+  <si>
+    <t>Sign and Keep open</t>
   </si>
 </sst>
 </file>
@@ -380,7 +404,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -417,12 +441,51 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>